<commit_message>
my account and admin panel test case written
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/server_list/server_list.xlsx
+++ b/apps/features/backlog/desktop/windows/server_list/server_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\server_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903B35C5-748E-4CC3-AEE3-C42080A356A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDC9991-2777-4011-A7E8-C12BE39D605E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="131">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -53,22 +53,10 @@
 2. User logged in.</t>
   </si>
   <si>
-    <t>Verify that the user can select a preferred server for the VPN connection.</t>
-  </si>
-  <si>
-    <t>Will establish the VPN connection with the selected server, display the connected status, and indicate the selected server.</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>TC_SYM_SP_002</t>
-  </si>
-  <si>
-    <t>Verify that the server page displays the list of available VPN servers.</t>
-  </si>
-  <si>
-    <t>The server page displays the list of available VPN servers.</t>
   </si>
   <si>
     <t>TC_SYM_SP_003</t>
@@ -77,9 +65,6 @@
     <t>1. VPN app installed and launched.
 2. User logged in.
 3. Currently viewing the server selection screen.</t>
-  </si>
-  <si>
-    <t>Verify that the search functionality works as expected, accurately displaying the matching server.</t>
   </si>
   <si>
     <t>should filter and search for specific VPN servers.</t>
@@ -93,21 +78,12 @@
 3.The user is on the server selection screen</t>
   </si>
   <si>
-    <t>Verify that the VPN app successfully disconnects to a gaming server.</t>
-  </si>
-  <si>
-    <t>The servers should be displayed in ascending order based on their names.</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_005</t>
   </si>
   <si>
     <t>1. VPN app installed and launched.
 2. User logged in.
 3. The device has a stable internet connection.</t>
-  </si>
-  <si>
-    <t>Verify that the VPN app successfully connects to a server.</t>
   </si>
   <si>
     <t>should establish a connection to the specified gaming server.</t>
@@ -122,34 +98,16 @@
     <t>TC_SYM_SP_007</t>
   </si>
   <si>
-    <t>High-Speed Server List Retrieval</t>
-  </si>
-  <si>
-    <t>The VPN app should offer a high-speed server list, display ratings, enable connection, and update the interface with selected server details.</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_008</t>
   </si>
   <si>
-    <t>Verify Ad-Blocking Server List Functionality</t>
-  </si>
-  <si>
-    <t>The VPN app should offer a customizable ad-blocking server list, ensuring effective ad blocking based on user preferences.</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_009</t>
-  </si>
-  <si>
-    <t>Verify Display of Gaming Server List</t>
   </si>
   <si>
     <t>The VPN app should offer a diverse gaming server list, enable server selection, establish connections</t>
   </si>
   <si>
     <t>TC_SYM_SP_010</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Verify Availability of Streaming Servers</t>
   </si>
   <si>
     <t>The VPN app should offer a streaming server list, enable user selection, and establish a seamless connection for content streaming.</t>
@@ -161,9 +119,6 @@
     <t>1.The VPN app is installed and operational.
 2.The user is logged in to the VPN app.
 3. The app contains multiple servers with distinct names.</t>
-  </si>
-  <si>
-    <t>Verify Searching Servers by Server Name</t>
   </si>
   <si>
     <t>The app should accurately find and display servers by the entered name, handling invalid server names appropriately.</t>
@@ -197,9 +152,6 @@
     <t>TC_SYM_SP_013</t>
   </si>
   <si>
-    <t>Ensure connection limit is enforced</t>
-  </si>
-  <si>
     <t>1.The VPN app is installed on three devices.
 2. All devices are set up to connect to the same server.
 3. The PIN for the server is the same on all devices.</t>
@@ -219,9 +171,6 @@
     <t>Device 4 should not be able to connect.</t>
   </si>
   <si>
-    <t>Verify PIN validation</t>
-  </si>
-  <si>
     <t>1. The VPN app is installed on four devices.
 2. All devices are set up to connect to the same server.
 3. The PIN for the server is different on each device.</t>
@@ -231,9 +180,6 @@
   </si>
   <si>
     <t>All devices should be able to connect successfully.</t>
-  </si>
-  <si>
-    <t>Scenario : Server Page</t>
   </si>
   <si>
     <t>TC_SYM_SP_016</t>
@@ -368,93 +314,10 @@
     <t>1. Go to appstore and install SymlexVPN in the desktop
 2. Open the installed SymlexVPN Application.
 3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. Select a server from the available list.
-6. Click on the "Connect" button.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the server page.
-5. Verify that the list of VPN servers is displayed.
-6. Verify that each server entry includes relevant information such as server name, location, and connection status.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the server page.
-5. Use the search functionality to search for "Singapore-3" servers.
-6. Verify that the search functionality works as expected, accurately displaying the matching server.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the server selection screen.
-5. Note down the order of the servers displayed..
-6. Verify that the search functionality works as expected, accurately displaying the matching server.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. Select a server from the available list.
-6. Click on the "Connect" button.
-7. Wait for the app to establish a connection.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the server selection section.
-5.Locate and select the "High-Speed Servers" option.
-6. Confirm that each server in the list is marked with its corresponding speed rating.
-7. Select a server from the high-speed list.
-8. Verify that the connection to the chosen high-speed server is established successfully.
-9. Check the app's interface to ensure it reflects the updated server information, including the selected high-speed server.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the server selection section.
-5. Locate and select the "Ad- blocking Servers" option.
-6. Click on that server to connect
-7. Test the ad-blocking functionality by accessing a website with known ads.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Verify that the gaming server list is displayed.
-5.Check if the gaming server list includes popular gaming servers or specific gaming regions.
-6. Select a gaming server from the list.
-7. Confirm that the app indicates the selected gaming server.
-8. Attempt to establish a connection to the selected gaming server.
-9.Verify that the connection is successful and the app displays the connected status.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
 4. Verify that the Streaming server list is displayed.
 5. Select a streaming server from the list.
 6. Attempt to connect to the selected streaming server.
 7. Open a streaming service and attempt to stream content.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. Navigate to the server search functionality.
-6.Enter the name of an existing server in the search bar.
-7. Verify that the app displays the searched server in the results.
-8. Confirm that the displayed server details match the entered server name.
-9. Repeat the process with an invalid server name to ensure the search functionality accurately handles non-existent servers.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Go to appstore and install SymlexVPN in the desktop
@@ -463,14 +326,6 @@
 4. Navigate to the VPN connection page.
 5.  Enter the PIN and attempt to connect to the server.
 7.  Repeat steps 1-2 for Devices 2, 3. </t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials on device 1
-4. Navigate to the VPN connection page.
-5.  Enter the PIN and attempt to connect to the server.
-7.  Repeat steps 1-2 for Devices 2, 3, and 4.</t>
   </si>
   <si>
     <t>1. Go to appstore and install SymlexVPN in the desktop
@@ -570,6 +425,154 @@
 3. Login with proper credentials
 4. Navigate to the VPN connection page.
 5. simulate a high number of users connecting to servers simultaneously</t>
+  </si>
+  <si>
+    <t>Test Scenario : Server Page</t>
+  </si>
+  <si>
+    <t>verify that the user can select a preferred server for the vpn connection.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page.
+5. select a server from the available list.
+6. click on the "Connect" button.</t>
+  </si>
+  <si>
+    <t>verify that the server page displays the list of available vpn servers.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page.
+5. verify that the list of vpn servers is displayed.
+6. verify that each server entry includes relevant information such as server name, location, and connection status.</t>
+  </si>
+  <si>
+    <t>the server page displays the list of available vpn servers.</t>
+  </si>
+  <si>
+    <t>Will establish the vpn connection with the selected server, display the connected status, and indicate the selected server.</t>
+  </si>
+  <si>
+    <t>verify that the search functionality works as expected, accurately displaying the matching server.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page.
+5. select a server from the available list.
+6. click on the "connect" button.
+7. wait for the app to establish a connection.</t>
+  </si>
+  <si>
+    <t>verify that the vpn app successfully connects to a server.</t>
+  </si>
+  <si>
+    <t>verify that the vpn app successfully disconnects to a gaming server.</t>
+  </si>
+  <si>
+    <t>high-speed server list retrieval</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server selection section.
+5. locate and select the "high-speed servers" option.
+6. confirm that each server in the list is marked with its corresponding speed rating.
+7. select a server from the high-speed list.
+8. verify that the connection to the chosen high-speed server is established successfully.
+9. check the app's interface to ensure it reflects the updated server information, including the selected high-speed server.</t>
+  </si>
+  <si>
+    <t>the vpn app should offer a high-speed server list, display ratings, enable connection, and update the interface with selected server details.</t>
+  </si>
+  <si>
+    <t>verify ad-blocking server list functionality</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server selection section.
+5. locate and select the "ad- blocking servers" option.
+6. click on that server to connect
+7. test the ad-blocking functionality by accessing a website with known ads.</t>
+  </si>
+  <si>
+    <t>The vpn app should offer a customizable ad-blocking server list, ensuring effective ad blocking based on user preferences.</t>
+  </si>
+  <si>
+    <t>verify display of gaming server list</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn Application.
+3. login with proper credentials
+4. navigate to the server page
+5. use the search functionality to search for "Singapore-3" servers.
+6. verify that the search functionality works as expected, accurately displaying the matching server.</t>
+  </si>
+  <si>
+    <t>the servers should disconnect successfully</t>
+  </si>
+  <si>
+    <t>verify that the vpn app successfully disconnects to a ad blocking server</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application
+3. login with proper credentials
+4. navigate to the server selection screen
+5. note down the order of the servers displayed
+6. verify that the vpn app successfully disconnects to a ad blocking server</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn  application.
+3. Login with proper credentials
+4. Verify that the gaming server list is displayed.
+5.Check if the gaming server list includes popular gaming servers or specific gaming regions.
+6. Select a gaming server from the list.
+7. Confirm that the app indicates the selected gaming server.
+8. attempt to establish a connection to the selected gaming server.
+9.verify that the connection is successful and the app displays the connected status.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verify availability of streaming servers</t>
+  </si>
+  <si>
+    <t>check to verify searching servers by server name</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install SymlexVPN in the desktop
+2. open the installed SymlexVPN Application.
+3. Login with proper credentials
+4. Navigate to the VPN connection page.
+5. Navigate to the server search functionality.
+6.Enter the name of an existing server in the search bar.
+7. Verify that the app displays the searched server in the results.
+8. Confirm that the displayed server details match the entered server name.
+9. Repeat the process with an invalid server name to ensure the search functionality accurately handles non-existent servers.</t>
+  </si>
+  <si>
+    <t>ensure connection limit is enforced</t>
+  </si>
+  <si>
+    <t>Verify pin validation</t>
+  </si>
+  <si>
+    <t>1. Go to appstore and install SymlexVPN in the desktop
+2. Open the installed SymlexVPN Application.
+3. Login with proper credentials on device 1
+4.  Navigate to the VPN connection page.
+5.  Enter the PIN and attempt to connect to the server.
+7.  Repeat steps 1-2 for Devices 2, 3, and 4.</t>
   </si>
 </sst>
 </file>
@@ -802,14 +805,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -837,6 +832,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1409,15 +1412,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G31" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G31" dataDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1627,8 +1630,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1644,15 +1647,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>62</v>
+      <c r="A1" s="20" t="s">
+        <v>102</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1674,13 +1677,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1744,25 +1747,25 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="5"/>
@@ -1787,22 +1790,22 @@
     </row>
     <row r="5" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="5"/>
@@ -1827,22 +1830,22 @@
     </row>
     <row r="6" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
@@ -1865,24 +1868,24 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
@@ -1907,22 +1910,22 @@
     </row>
     <row r="8" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="5"/>
@@ -1945,26 +1948,26 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" ht="108.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>28</v>
+    <row r="9" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>20</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>25</v>
+      <c r="B9" s="12" t="s">
+        <v>18</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>22</v>
+      <c r="C9" s="12" t="s">
+        <v>112</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>108</v>
+      <c r="D9" s="12" t="s">
+        <v>110</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>29</v>
+      <c r="E9" s="12" t="s">
+        <v>21</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>12</v>
+      <c r="F9" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1986,25 +1989,25 @@
       <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="204" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>30</v>
+      <c r="A10" s="13" t="s">
+        <v>22</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>25</v>
+      <c r="B10" s="12" t="s">
+        <v>18</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>31</v>
+      <c r="C10" s="12" t="s">
+        <v>113</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>109</v>
+      <c r="D10" s="12" t="s">
+        <v>114</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>32</v>
+      <c r="E10" s="12" t="s">
+        <v>115</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>12</v>
+      <c r="F10" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -2026,25 +2029,25 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>33</v>
+      <c r="A11" s="13" t="s">
+        <v>23</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>25</v>
+      <c r="B11" s="12" t="s">
+        <v>18</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>34</v>
+      <c r="C11" s="13" t="s">
+        <v>116</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>110</v>
+      <c r="D11" s="12" t="s">
+        <v>117</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>35</v>
+      <c r="E11" s="12" t="s">
+        <v>118</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>12</v>
+      <c r="F11" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2066,25 +2069,25 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="199.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>36</v>
+      <c r="A12" s="13" t="s">
+        <v>24</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>37</v>
+      <c r="F12" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2106,25 +2109,25 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>39</v>
+      <c r="A13" s="13" t="s">
+        <v>26</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>25</v>
+      <c r="B13" s="12" t="s">
+        <v>18</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>40</v>
+      <c r="C13" s="13" t="s">
+        <v>125</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>112</v>
+      <c r="D13" s="12" t="s">
+        <v>86</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>41</v>
+      <c r="E13" s="12" t="s">
+        <v>27</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>12</v>
+      <c r="F13" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2146,25 +2149,25 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="196.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>42</v>
+      <c r="A14" s="13" t="s">
+        <v>28</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>43</v>
+      <c r="B14" s="12" t="s">
+        <v>29</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>44</v>
+      <c r="C14" s="13" t="s">
+        <v>126</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>113</v>
+      <c r="D14" s="12" t="s">
+        <v>127</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>45</v>
+      <c r="E14" s="12" t="s">
+        <v>30</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>12</v>
+      <c r="F14" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2185,26 +2188,26 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="168" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>46</v>
+    <row r="15" spans="1:26" ht="219" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>31</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>47</v>
+      <c r="B15" s="16" t="s">
+        <v>32</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>48</v>
+      <c r="C15" s="15" t="s">
+        <v>33</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>49</v>
+      <c r="D15" s="16" t="s">
+        <v>34</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>50</v>
+      <c r="E15" s="16" t="s">
+        <v>35</v>
       </c>
-      <c r="F15" s="22" t="s">
-        <v>12</v>
+      <c r="F15" s="16" t="s">
+        <v>10</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2226,25 +2229,25 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="116.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
-        <v>51</v>
+      <c r="A16" s="15" t="s">
+        <v>36</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>53</v>
+      <c r="B16" s="16" t="s">
+        <v>37</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>52</v>
+      <c r="C16" s="15" t="s">
+        <v>128</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>114</v>
+      <c r="D16" s="16" t="s">
+        <v>87</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>54</v>
+      <c r="E16" s="15" t="s">
+        <v>38</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>12</v>
+      <c r="F16" s="16" t="s">
+        <v>10</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -2266,25 +2269,25 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>55</v>
+      <c r="A17" s="13" t="s">
+        <v>39</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>56</v>
+      <c r="B17" s="12" t="s">
+        <v>40</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>52</v>
+      <c r="C17" s="13" t="s">
+        <v>128</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>115</v>
+      <c r="D17" s="12" t="s">
+        <v>130</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>57</v>
+      <c r="E17" s="13" t="s">
+        <v>41</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>12</v>
+      <c r="F17" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2306,25 +2309,25 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
-        <v>60</v>
+      <c r="A18" s="13" t="s">
+        <v>43</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>59</v>
+      <c r="B18" s="12" t="s">
+        <v>42</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>58</v>
+      <c r="C18" s="13" t="s">
+        <v>129</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>116</v>
+      <c r="D18" s="12" t="s">
+        <v>88</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>61</v>
+      <c r="E18" s="14" t="s">
+        <v>44</v>
       </c>
-      <c r="F18" s="18" t="s">
-        <v>12</v>
+      <c r="F18" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2346,25 +2349,25 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>63</v>
+      <c r="A19" s="13" t="s">
+        <v>45</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>68</v>
+      <c r="B19" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>64</v>
+      <c r="C19" s="13" t="s">
+        <v>46</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>117</v>
+      <c r="D19" s="12" t="s">
+        <v>89</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>65</v>
+      <c r="E19" s="12" t="s">
+        <v>47</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>12</v>
+      <c r="F19" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="G19" s="19"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2386,23 +2389,23 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
-        <v>67</v>
+      <c r="A20" s="13" t="s">
+        <v>49</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>68</v>
+      <c r="B20" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>66</v>
+      <c r="C20" s="17" t="s">
+        <v>48</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>118</v>
+      <c r="D20" s="12" t="s">
+        <v>90</v>
       </c>
-      <c r="E20" s="23" t="s">
-        <v>69</v>
+      <c r="E20" s="17" t="s">
+        <v>51</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2424,23 +2427,23 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
-        <v>70</v>
+      <c r="A21" s="15" t="s">
+        <v>52</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>68</v>
+      <c r="B21" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C21" s="24" t="s">
-        <v>71</v>
+      <c r="C21" s="18" t="s">
+        <v>53</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>119</v>
+      <c r="D21" s="12" t="s">
+        <v>91</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>72</v>
+      <c r="E21" s="18" t="s">
+        <v>54</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2462,23 +2465,23 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
-        <v>73</v>
+      <c r="A22" s="15" t="s">
+        <v>55</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>68</v>
+      <c r="B22" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C22" s="23" t="s">
-        <v>74</v>
+      <c r="C22" s="17" t="s">
+        <v>56</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>120</v>
+      <c r="D22" s="12" t="s">
+        <v>92</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>75</v>
+      <c r="E22" s="17" t="s">
+        <v>57</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2500,23 +2503,23 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
-        <v>76</v>
+      <c r="A23" s="15" t="s">
+        <v>58</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>68</v>
+      <c r="B23" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C23" s="23" t="s">
-        <v>77</v>
+      <c r="C23" s="17" t="s">
+        <v>59</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>121</v>
+      <c r="D23" s="12" t="s">
+        <v>93</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>79</v>
+      <c r="E23" s="17" t="s">
+        <v>61</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2538,23 +2541,23 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>81</v>
+      <c r="A24" s="15" t="s">
+        <v>63</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>68</v>
+      <c r="B24" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C24" s="23" t="s">
-        <v>78</v>
+      <c r="C24" s="17" t="s">
+        <v>60</v>
       </c>
-      <c r="D24" s="18" t="s">
-        <v>122</v>
+      <c r="D24" s="12" t="s">
+        <v>94</v>
       </c>
-      <c r="E24" s="23" t="s">
-        <v>80</v>
+      <c r="E24" s="17" t="s">
+        <v>62</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2576,25 +2579,25 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
-        <v>83</v>
+      <c r="A25" s="15" t="s">
+        <v>65</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" s="23"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2616,23 +2619,23 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
-        <v>88</v>
+      <c r="A26" s="15" t="s">
+        <v>70</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>68</v>
+      <c r="B26" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C26" s="23" t="s">
-        <v>84</v>
+      <c r="C26" s="17" t="s">
+        <v>66</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>124</v>
+      <c r="D26" s="12" t="s">
+        <v>96</v>
       </c>
-      <c r="E26" s="25" t="s">
-        <v>85</v>
+      <c r="E26" s="19" t="s">
+        <v>67</v>
       </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2654,23 +2657,23 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
-        <v>91</v>
+      <c r="A27" s="15" t="s">
+        <v>73</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>68</v>
+      <c r="B27" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C27" s="23" t="s">
-        <v>89</v>
+      <c r="C27" s="17" t="s">
+        <v>71</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>125</v>
+      <c r="D27" s="12" t="s">
+        <v>97</v>
       </c>
-      <c r="E27" s="23" t="s">
-        <v>90</v>
+      <c r="E27" s="17" t="s">
+        <v>72</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2692,23 +2695,23 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
-        <v>93</v>
+      <c r="A28" s="15" t="s">
+        <v>75</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>68</v>
+      <c r="B28" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C28" s="23" t="s">
-        <v>92</v>
+      <c r="C28" s="17" t="s">
+        <v>74</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>126</v>
+      <c r="D28" s="12" t="s">
+        <v>98</v>
       </c>
-      <c r="E28" s="23" t="s">
-        <v>94</v>
+      <c r="E28" s="17" t="s">
+        <v>76</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2730,23 +2733,23 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
-        <v>96</v>
+      <c r="A29" s="15" t="s">
+        <v>78</v>
       </c>
-      <c r="B29" s="18" t="s">
-        <v>68</v>
+      <c r="B29" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>95</v>
+      <c r="C29" s="17" t="s">
+        <v>77</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>127</v>
+      <c r="D29" s="12" t="s">
+        <v>99</v>
       </c>
-      <c r="E29" s="23" t="s">
-        <v>97</v>
+      <c r="E29" s="17" t="s">
+        <v>79</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2768,23 +2771,23 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="s">
-        <v>98</v>
+      <c r="A30" s="15" t="s">
+        <v>80</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>68</v>
+      <c r="B30" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>99</v>
+      <c r="C30" s="17" t="s">
+        <v>81</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" s="23" t="s">
+      <c r="D30" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+      <c r="E30" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -2806,23 +2809,23 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
-        <v>102</v>
+      <c r="A31" s="15" t="s">
+        <v>84</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>68</v>
+      <c r="B31" s="12" t="s">
+        <v>50</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>129</v>
+      <c r="E31" s="17" t="s">
+        <v>85</v>
       </c>
-      <c r="E31" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>

</xml_diff>

<commit_message>
created and reviewed the test cases for kill switch(39) and executed server list test cases for enter vpn
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/server_list/server_list.xlsx
+++ b/apps/features/backlog/desktop/windows/server_list/server_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\server_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDC9991-2777-4011-A7E8-C12BE39D605E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96943F73-A8C9-4FC1-9E8D-0DDD3471AA09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="124">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -49,10 +49,6 @@
     <t>TC_SYM_SP_001</t>
   </si>
   <si>
-    <t>1. VPN app installed and launched.
-2. User logged in.</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -62,28 +58,10 @@
     <t>TC_SYM_SP_003</t>
   </si>
   <si>
-    <t>1. VPN app installed and launched.
-2. User logged in.
-3. Currently viewing the server selection screen.</t>
-  </si>
-  <si>
-    <t>should filter and search for specific VPN servers.</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_004</t>
   </si>
   <si>
-    <t>1.The VPN app is installed and operational.
-2.The user is logged in to the VPN app.
-3.The user is on the server selection screen</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_005</t>
-  </si>
-  <si>
-    <t>1. VPN app installed and launched.
-2. User logged in.
-3. The device has a stable internet connection.</t>
   </si>
   <si>
     <t>should establish a connection to the specified gaming server.</t>
@@ -104,21 +82,10 @@
     <t>TC_SYM_SP_009</t>
   </si>
   <si>
-    <t>The VPN app should offer a diverse gaming server list, enable server selection, establish connections</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_010</t>
   </si>
   <si>
-    <t>The VPN app should offer a streaming server list, enable user selection, and establish a seamless connection for content streaming.</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_011</t>
-  </si>
-  <si>
-    <t>1.The VPN app is installed and operational.
-2.The user is logged in to the VPN app.
-3. The app contains multiple servers with distinct names.</t>
   </si>
   <si>
     <t>The app should accurately find and display servers by the entered name, handling invalid server names appropriately.</t>
@@ -127,59 +94,13 @@
     <t>TC_SYM_SP_012</t>
   </si>
   <si>
-    <t>1.The VPN app is installed and operational.
-2.The user is logged in to the VPN app.
-3. The app contains servers categorized by different countries.</t>
-  </si>
-  <si>
-    <t>Verify Searching Servers by country Name</t>
-  </si>
-  <si>
-    <t>1. Go to Playstore and install SymlexVPN in the mobile.
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. Navigate to the server search functionality.
-6. Enter the name of an existing country in the search bar.
-7. Verify that the app displays servers associated with the entered country in the search results.
-8. Confirm that the displayed server details match the entered server name.
-9.Repeat the process with an invalid country name to ensure the search functionality handles non-existent countries accurately.</t>
-  </si>
-  <si>
-    <t>The app should accurately find and display servers by the entered name, handling invalid country names appropriately.</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_013</t>
-  </si>
-  <si>
-    <t>1.The VPN app is installed on three devices.
-2. All devices are set up to connect to the same server.
-3. The PIN for the server is the same on all devices.</t>
-  </si>
-  <si>
-    <t>Devices 1, 2, and 3 should connect successfully.</t>
   </si>
   <si>
     <t>TC_SYM_SP_014</t>
   </si>
   <si>
-    <t>1.The VPN app is installed on 4 devices.
-2. All devices are set up to connect to the same server.
-3. The PIN for the server is the same on all devices.</t>
-  </si>
-  <si>
-    <t>Device 4 should not be able to connect.</t>
-  </si>
-  <si>
-    <t>1. The VPN app is installed on four devices.
-2. All devices are set up to connect to the same server.
-3. The PIN for the server is different on each device.</t>
-  </si>
-  <si>
     <t>TC_SYM_SP_015</t>
-  </si>
-  <si>
-    <t>All devices should be able to connect successfully.</t>
   </si>
   <si>
     <t>TC_SYM_SP_016</t>
@@ -196,11 +117,6 @@
   </si>
   <si>
     <t>TC_SYM_SP_017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.The VPN app is installed on 4 devices.
-2. All devices are set up to connect to the same server.
-</t>
   </si>
   <si>
     <t>server should be consistently displayed</t>
@@ -251,16 +167,8 @@
     <t>check connection limitations</t>
   </si>
   <si>
-    <t>should confirm that the application enforces any
- connection limitations (e.g., one connection at a time)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t>should verify that only servers with high availability
- are listed</t>
   </si>
   <si>
     <t>TC_SYM_SP_023</t>
@@ -311,122 +219,6 @@
     <t>verify that the servers maintain their performance under increased load</t>
   </si>
   <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Verify that the Streaming server list is displayed.
-5. Select a streaming server from the list.
-6. Attempt to connect to the selected streaming server.
-7. Open a streaming service and attempt to stream content.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials on device 1
-4. Navigate to the VPN connection page.
-5.  Enter the PIN and attempt to connect to the server.
-7.  Repeat steps 1-2 for Devices 2, 3. </t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials on device 1
-4. Navigate to the VPN connection page.
-5. Enter a valid PIN and attempt to connect to the server.
-7. Repeat steps 1-2 for Devices 2, 3, and 4 using different valid PINs.</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page. 
-5. try to check visibility of server list</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. try to check that the server list consistently displays the available servers without any missing or duplicated entries</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. connect to a server from the list and observe if the server list dynamically updates to reflect the current connection status</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. test the sorting functionality for the server list (e.g., alphabetical order, by location, by speed)</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-6. test the filtering feature to display servers from a specific region</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. test the filtering feature to display servers based on types (e.g., standard, gaming, ad-blocking).</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page. 
-5. try to check the availability status of each server in the list</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. attempt to connect to multiple servers simultaneously</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. test the behavior when attempting to connect to a server that is temporarily offline</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. check for status indicators (e.g., online, offline) next to each server in the list</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. verify that servers in the list have speed labels indicating their performance (e.g., high-speed, standard)</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. connect to servers using different network types (e.g., 3G, 4G, Wi-Fi)</t>
-  </si>
-  <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. simulate a high number of users connecting to servers simultaneously</t>
-  </si>
-  <si>
     <t>Test Scenario : Server Page</t>
   </si>
   <si>
@@ -455,22 +247,7 @@
     <t>the server page displays the list of available vpn servers.</t>
   </si>
   <si>
-    <t>Will establish the vpn connection with the selected server, display the connected status, and indicate the selected server.</t>
-  </si>
-  <si>
     <t>verify that the search functionality works as expected, accurately displaying the matching server.</t>
-  </si>
-  <si>
-    <t>1. go to appstore and install symlexvpn in the desktop
-2. open the installed symlexvpn application.
-3. login with proper credentials
-4. navigate to the vpn connection page.
-5. select a server from the available list.
-6. click on the "connect" button.
-7. wait for the app to establish a connection.</t>
-  </si>
-  <si>
-    <t>verify that the vpn app successfully connects to a server.</t>
   </si>
   <si>
     <t>verify that the vpn app successfully disconnects to a gaming server.</t>
@@ -479,30 +256,10 @@
     <t>high-speed server list retrieval</t>
   </si>
   <si>
-    <t>1. go to appstore and install symlexvpn in the desktop
-2. open the installed symlexvpn application.
-3. login with proper credentials
-4. navigate to the server selection section.
-5. locate and select the "high-speed servers" option.
-6. confirm that each server in the list is marked with its corresponding speed rating.
-7. select a server from the high-speed list.
-8. verify that the connection to the chosen high-speed server is established successfully.
-9. check the app's interface to ensure it reflects the updated server information, including the selected high-speed server.</t>
-  </si>
-  <si>
     <t>the vpn app should offer a high-speed server list, display ratings, enable connection, and update the interface with selected server details.</t>
   </si>
   <si>
     <t>verify ad-blocking server list functionality</t>
-  </si>
-  <si>
-    <t>1. go to appstore and install symlexvpn in the desktop
-2. open the installed symlexvpn application.
-3. login with proper credentials
-4. navigate to the server selection section.
-5. locate and select the "ad- blocking servers" option.
-6. click on that server to connect
-7. test the ad-blocking functionality by accessing a website with known ads.</t>
   </si>
   <si>
     <t>The vpn app should offer a customizable ad-blocking server list, ensuring effective ad blocking based on user preferences.</t>
@@ -511,68 +268,276 @@
     <t>verify display of gaming server list</t>
   </si>
   <si>
-    <t>1. go to appstore and install symlexvpn in the desktop
-2. open the installed symlexvpn Application.
-3. login with proper credentials
-4. navigate to the server page
-5. use the search functionality to search for "Singapore-3" servers.
-6. verify that the search functionality works as expected, accurately displaying the matching server.</t>
-  </si>
-  <si>
-    <t>the servers should disconnect successfully</t>
-  </si>
-  <si>
-    <t>verify that the vpn app successfully disconnects to a ad blocking server</t>
-  </si>
-  <si>
-    <t>1. go to appstore and install symlexvpn in the desktop
-2. open the installed symlexvpn application
-3. login with proper credentials
-4. navigate to the server selection screen
-5. note down the order of the servers displayed
-6. verify that the vpn app successfully disconnects to a ad blocking server</t>
-  </si>
-  <si>
-    <t>1. go to appstore and install symlexvpn in the desktop
-2. open the installed symlexvpn  application.
-3. Login with proper credentials
-4. Verify that the gaming server list is displayed.
-5.Check if the gaming server list includes popular gaming servers or specific gaming regions.
-6. Select a gaming server from the list.
-7. Confirm that the app indicates the selected gaming server.
-8. attempt to establish a connection to the selected gaming server.
-9.verify that the connection is successful and the app displays the connected status.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> verify availability of streaming servers</t>
   </si>
   <si>
     <t>check to verify searching servers by server name</t>
   </si>
   <si>
-    <t>1. go to appstore and install SymlexVPN in the desktop
-2. open the installed SymlexVPN Application.
-3. Login with proper credentials
-4. Navigate to the VPN connection page.
-5. Navigate to the server search functionality.
-6.Enter the name of an existing server in the search bar.
-7. Verify that the app displays the searched server in the results.
-8. Confirm that the displayed server details match the entered server name.
-9. Repeat the process with an invalid server name to ensure the search functionality accurately handles non-existent servers.</t>
+    <t>verify that the vpn app successfully connects to a ad blocking server</t>
   </si>
   <si>
-    <t>ensure connection limit is enforced</t>
+    <t>verify that the vpn app successfully connects to a gaming server.</t>
   </si>
   <si>
-    <t>Verify pin validation</t>
+    <t>check to verify searching servers by country name</t>
   </si>
   <si>
-    <t>1. Go to appstore and install SymlexVPN in the desktop
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials on device 1
-4.  Navigate to the VPN connection page.
-5.  Enter the PIN and attempt to connect to the server.
-7.  Repeat steps 1-2 for Devices 2, 3, and 4.</t>
+    <t>check to verify pin validation</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install entervpn in the desktop
+2. open the installed entervpn application.
+3. login with proper credentials on device -1
+4. navigate to the server page
+5. attempt to connect to the server.
+6. repeat steps 1-5 for devices 2, 3, and 4 using different valid pins.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install entervpn in the desktop
+2. open the installed entervpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page. 
+5. test the sorting functionality for the server list (e.g., alphabetical order, by location, by speed)</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install entervpn in the desktop
+2. open the installed entervpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page
+5. test the filtering feature to display servers based on types (e.g., standard, gaming, ad-blocking)</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page
+5. simulate a high number of users connecting to servers simultaneously</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page
+5. connect to servers using different network types (e.g., 3G, 4G, Wi-Fi)</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page
+5. verify that servers in the list have speed labels indicating their performance (e.g., high-speed, standard)</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page
+5. check for status indicators (e.g., online, offline) next to each server in the list</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page
+5. test the behavior when attempting to connect to a server that is temporarily offline</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page. 
+5. attempt to connect to multiple servers simultaneously</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page
+5. try to check the availability status of each server in the list</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page. 
+5. test the filtering feature to display servers from a specific region</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page. 
+5. connect to a server from the list and observe if the server list dynamically updates to reflect the current connection status</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page. 
+5. try to check visibility of server list</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page. 
+5. try to check that the server list consistently displays the available servers without any missing or duplicated entries</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials on device -1
+4. navigate to the server page
+5. attempt to connect to the server.
+6. repeat steps 1-5 for Devices 2, 3, and 4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials on device -1
+4. navigate to the server page
+5. attempt to connect to the server.
+6. repeat steps 1-5 for Devices 2, 3. </t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page
+5. navigate to the server search functionality.
+6. enter the name of an existing server in the search bar.
+7. verify that the app displays the searched server in the results.
+8. confirm that the displayed server details match the entered server name.
+9. repeat the process with an invalid server name to ensure the search functionality accurately handles non-existent servers.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page
+5. navigate to the server search functionality.
+6. enter the name of an existing country in the search bar.
+7. verify that the app displays servers associated with the entered country in the search results.
+8. confirm that the displayed server details match the entered server name.
+9. repeat the process with an invalid country name to ensure the search functionality handles non-existent countries accurately.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page
+5.Check if the gaming server list includes popular gaming servers or specific gaming regions.
+6. confirm that the app indicates the selected gaming server.
+7. attempt to establish a connection to the selected gaming server.
+8.verify that the connection is successful and the app displays the connected status.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page
+5. verify that the streaming server list is displayed.
+6. select a streaming server from the list.
+7. attempt to connect to the selected streaming server.
+8. open a streaming service and attempt to stream content.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page
+5. locate and select the "ad- blocking servers" option.
+6. click on that server to connect
+7. test the ad-blocking functionality by accessing a website with known ads.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page
+5. locate and select the "high-speed servers" option.
+6. confirm that each server in the list is marked with its corresponding speed rating.
+7. select a server from the high-speed list.
+8. verify that the connection to the chosen high-speed server is established successfully.
+9. check the app's interface to ensure it reflects the updated server information, including the selected high-speed server.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page.
+5. select a gaming server from the available list.
+6. click on the "connect" button.
+7. wait for the app to establish a connection.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page.
+5. disconnect the connected gaming server</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page.
+5. use the search functionality to search servers.
+6. verify that the search functionality works as expected, accurately displaying the matching server.</t>
+  </si>
+  <si>
+    <t>1. go to appstore and install symlexvpn in the desktop
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the server page.
+5. note down the order of the servers displayed
+6. verify that the vpn app successfully connects to a ad blocking server</t>
+  </si>
+  <si>
+    <t>will establish the vpn connection with the selected server, display the connected status, and indicate the selected server.</t>
+  </si>
+  <si>
+    <t>should filter and search for specific vpn servers.</t>
+  </si>
+  <si>
+    <t>the servers should connect successfully</t>
+  </si>
+  <si>
+    <t>The vpn app should offer a diverse gaming server list, enable server selection, establish connections</t>
+  </si>
+  <si>
+    <t>The vpn app should offer a streaming server list, enable user selection, and establish a seamless connection for content streaming.</t>
+  </si>
+  <si>
+    <t>the app should accurately find and display servers by the entered name, handling invalid country names appropriately.</t>
+  </si>
+  <si>
+    <t>devices 1, 2, and 3 should connect successfully.</t>
+  </si>
+  <si>
+    <t>device 4 should not be able to connect.</t>
+  </si>
+  <si>
+    <t>all devices should be able to connect successfully.</t>
+  </si>
+  <si>
+    <t>should verify that only servers with high availability are listed</t>
+  </si>
+  <si>
+    <t>should confirm that the application enforces any
+connection limitations (e.g., one connection at a time)</t>
+  </si>
+  <si>
+    <t>1. vpn app installed and launched.
+2. user logged in.
+3. the device has a stable internet connection.</t>
+  </si>
+  <si>
+    <t>check connection limit for three device</t>
+  </si>
+  <si>
+    <t>check connection limit for four device</t>
   </si>
 </sst>
 </file>
@@ -647,7 +612,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -773,11 +738,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -832,6 +810,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -875,8 +862,28 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -886,8 +893,28 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -897,8 +924,28 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -908,8 +955,28 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1630,8 +1697,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1647,15 +1714,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>102</v>
+      <c r="A1" s="23" t="s">
+        <v>65</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1677,13 +1744,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1708,16 +1775,16 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1750,20 +1817,20 @@
       <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>9</v>
+      <c r="B4" s="12" t="s">
+        <v>121</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>103</v>
+      <c r="C4" s="20" t="s">
+        <v>66</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>104</v>
+      <c r="D4" s="20" t="s">
+        <v>67</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>108</v>
+      <c r="E4" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>7</v>
@@ -1790,22 +1857,22 @@
     </row>
     <row r="5" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>9</v>
+      <c r="B5" s="12" t="s">
+        <v>121</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>105</v>
+      <c r="C5" s="12" t="s">
+        <v>68</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>106</v>
+      <c r="D5" s="12" t="s">
+        <v>69</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>107</v>
+      <c r="E5" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="5"/>
@@ -1830,22 +1897,22 @@
     </row>
     <row r="6" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
+      <c r="B6" s="12" t="s">
+        <v>121</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>109</v>
+      <c r="C6" s="12" t="s">
+        <v>71</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>120</v>
+      <c r="D6" s="12" t="s">
+        <v>108</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>14</v>
+      <c r="E6" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
@@ -1870,22 +1937,22 @@
     </row>
     <row r="7" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="B7" s="12" t="s">
         <v>121</v>
       </c>
+      <c r="C7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>112</v>
+      </c>
       <c r="F7" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
@@ -1910,22 +1977,22 @@
     </row>
     <row r="8" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>18</v>
+      <c r="B8" s="12" t="s">
+        <v>121</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>111</v>
+      <c r="C8" s="12" t="s">
+        <v>81</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>110</v>
+      <c r="D8" s="12" t="s">
+        <v>106</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>19</v>
+      <c r="E8" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="5"/>
@@ -1950,22 +2017,22 @@
     </row>
     <row r="9" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="6"/>
@@ -1990,22 +2057,22 @@
     </row>
     <row r="10" spans="1:26" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="6"/>
@@ -2030,22 +2097,22 @@
     </row>
     <row r="11" spans="1:26" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="1"/>
@@ -2070,22 +2137,22 @@
     </row>
     <row r="12" spans="1:26" ht="199.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="1"/>
@@ -2108,24 +2175,24 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="1"/>
@@ -2150,22 +2217,22 @@
     </row>
     <row r="14" spans="1:26" ht="196.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="1"/>
@@ -2190,22 +2257,22 @@
     </row>
     <row r="15" spans="1:26" ht="219" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>32</v>
+      <c r="B15" s="12" t="s">
+        <v>121</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>33</v>
+      <c r="C15" s="13" t="s">
+        <v>82</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>34</v>
+      <c r="D15" s="12" t="s">
+        <v>101</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>35</v>
+      <c r="E15" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="1"/>
@@ -2230,22 +2297,22 @@
     </row>
     <row r="16" spans="1:26" ht="116.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>37</v>
+      <c r="B16" s="12" t="s">
+        <v>121</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>128</v>
+      <c r="C16" s="13" t="s">
+        <v>122</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>87</v>
+      <c r="D16" s="12" t="s">
+        <v>99</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>38</v>
+      <c r="E16" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="10"/>
@@ -2270,22 +2337,22 @@
     </row>
     <row r="17" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>41</v>
+      <c r="E17" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="1"/>
@@ -2310,22 +2377,22 @@
     </row>
     <row r="18" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>44</v>
+      <c r="E18" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="1"/>
@@ -2350,22 +2417,22 @@
     </row>
     <row r="19" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="1"/>
@@ -2390,19 +2457,19 @@
     </row>
     <row r="20" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>48</v>
+      <c r="C20" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>51</v>
+      <c r="E20" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -2428,19 +2495,19 @@
     </row>
     <row r="21" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>53</v>
+      <c r="C21" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>54</v>
+      <c r="E21" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -2466,19 +2533,19 @@
     </row>
     <row r="22" spans="1:26" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>56</v>
+      <c r="C22" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>57</v>
+      <c r="E22" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -2504,19 +2571,19 @@
     </row>
     <row r="23" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>59</v>
+      <c r="C23" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>61</v>
+      <c r="E23" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -2542,19 +2609,19 @@
     </row>
     <row r="24" spans="1:26" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>60</v>
+      <c r="C24" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>62</v>
+      <c r="E24" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -2580,22 +2647,22 @@
     </row>
     <row r="25" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>64</v>
+      <c r="C25" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>69</v>
+      <c r="E25" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="1"/>
@@ -2620,19 +2687,19 @@
     </row>
     <row r="26" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>66</v>
+      <c r="C26" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>67</v>
+      <c r="E26" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -2658,19 +2725,19 @@
     </row>
     <row r="27" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>71</v>
+      <c r="D27" s="12" t="s">
+        <v>91</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>72</v>
+      <c r="E27" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
@@ -2696,19 +2763,19 @@
     </row>
     <row r="28" spans="1:26" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>74</v>
+      <c r="C28" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>76</v>
+      <c r="E28" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
@@ -2734,19 +2801,19 @@
     </row>
     <row r="29" spans="1:26" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>77</v>
+      <c r="C29" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>79</v>
+      <c r="E29" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
@@ -2772,19 +2839,19 @@
     </row>
     <row r="30" spans="1:26" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>81</v>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>82</v>
+      <c r="E30" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
@@ -2810,19 +2877,19 @@
     </row>
     <row r="31" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>50</v>
+      <c r="B31" s="16" t="s">
+        <v>121</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>83</v>
+      <c r="C31" s="15" t="s">
+        <v>62</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>101</v>
+      <c r="D31" s="16" t="s">
+        <v>87</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>85</v>
+      <c r="E31" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="17"/>

</xml_diff>